<commit_message>
feat: :sparkles: JSON and Python import/export system
</commit_message>
<xml_diff>
--- a/tests/material/registers/xlsx/registers.xlsx
+++ b/tests/material/registers/xlsx/registers.xlsx
@@ -2,16 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="nominal" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="ordinal" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="numerical" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="date" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="object" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="computers" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -107,6 +109,63 @@
   </si>
   <si>
     <t xml:space="preserve">54-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car:brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car:model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car:fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car:year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toyota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corolla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gasoline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">renault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nissan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer:cpu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer:gpu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer:storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nvidia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">radeon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qualcom</t>
   </si>
 </sst>
 </file>
@@ -123,6 +182,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,12 +242,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -320,91 +388,94 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="b">
+      <c r="D2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="b">
+      <c r="D3" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="b">
+      <c r="D4" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -426,64 +497,64 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>12</v>
       </c>
     </row>
@@ -505,91 +576,91 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>0.65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>0.23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1.12</v>
       </c>
     </row>
@@ -611,8 +682,72 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>45058</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>53327</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,39 +757,155 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>45058</v>
+      <c r="B2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>44581</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>44270</v>
+      <c r="B3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>37400</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.17"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>512</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>53327</v>
+      <c r="B4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>512</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>46</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: :sparkles: Import data from .xlsx files
</commit_message>
<xml_diff>
--- a/tests/material/registers/xlsx/registers.xlsx
+++ b/tests/material/registers/xlsx/registers.xlsx
@@ -12,7 +12,7 @@
     <sheet name="ordinal" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="numerical" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="date" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="object" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="car" sheetId="5" state="visible" r:id="rId7"/>
     <sheet name="computers" sheetId="6" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -111,16 +111,16 @@
     <t xml:space="preserve">54-12</t>
   </si>
   <si>
-    <t xml:space="preserve">car:brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">car:model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">car:fuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">car:year</t>
+    <t xml:space="preserve">brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
   </si>
   <si>
     <t xml:space="preserve">toyota</t>
@@ -144,13 +144,13 @@
     <t xml:space="preserve">gas</t>
   </si>
   <si>
-    <t xml:space="preserve">computer:cpu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">computer:gpu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">computer:storage</t>
+    <t xml:space="preserve">cpu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gpu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage</t>
   </si>
   <si>
     <t xml:space="preserve">amd</t>
@@ -242,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,10 +256,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -747,67 +743,67 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="3" t="n">
         <v>44581</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="3" t="n">
         <v>37400</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -830,81 +826,81 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>512</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>512</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>512</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: :sparkles: Formula variables added
</commit_message>
<xml_diff>
--- a/tests/material/registers/xlsx/registers.xlsx
+++ b/tests/material/registers/xlsx/registers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="nominal" sheetId="1" state="visible" r:id="rId3"/>
@@ -572,8 +572,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -622,9 +622,7 @@
       <c r="C3" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>45</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1" t="n">
         <v>0.23</v>
       </c>
@@ -825,7 +823,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: :sparkles: Variable control inside a register added
</commit_message>
<xml_diff>
--- a/tests/material/registers/xlsx/registers.xlsx
+++ b/tests/material/registers/xlsx/registers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="nominal" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t xml:space="preserve">birth_day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">death_day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-56</t>
   </si>
   <si>
     <t xml:space="preserve">54-12</t>
@@ -242,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -256,6 +262,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -674,10 +684,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -689,6 +699,9 @@
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -697,6 +710,9 @@
       <c r="B2" s="3" t="n">
         <v>45058</v>
       </c>
+      <c r="C2" s="4" t="n">
+        <v>45444</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -705,6 +721,9 @@
       <c r="B3" s="3" t="n">
         <v>44270</v>
       </c>
+      <c r="C3" s="4" t="n">
+        <v>43954</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -713,13 +732,19 @@
       <c r="B4" s="3" t="n">
         <v>53327</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>35033</v>
       </c>
     </row>
   </sheetData>
@@ -751,16 +776,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,13 +793,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>44581</v>
@@ -785,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>37400</v>
@@ -796,13 +821,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -840,13 +865,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,10 +879,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>512</v>
@@ -868,10 +893,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>512</v>
@@ -882,10 +907,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>512</v>
@@ -896,10 +921,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>